<commit_message>
Exported shocked tables for each scenario and refined linkages calculation
</commit_message>
<xml_diff>
--- a/Paths.xlsx
+++ b/Paths.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\SESAM\GT-IOA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1668F8C9-B4C7-4315-ACFD-4084537B76B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3572BBCD-F38E-4ED7-BBCF-BD95F8E7CC09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>LR</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>C:\Users\loren\Documents\GitHub\SESAM\GT-IOA\Results</t>
+  </si>
+  <si>
+    <t>Plots</t>
+  </si>
+  <si>
+    <t>C:\Users\loren\Documents\GitHub\SESAM\GT-IOA\Plots</t>
   </si>
 </sst>
 </file>
@@ -99,8 +105,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -381,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,6 +453,17 @@
         <v>12</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
sensitivity analysis set up
</commit_message>
<xml_diff>
--- a/Paths.xlsx
+++ b/Paths.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\SESAM\GT-IOA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3572BBCD-F38E-4ED7-BBCF-BD95F8E7CC09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D49993F-94A0-4C1B-A88C-24DF4DEF2DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,20 +25,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>LR</t>
   </si>
   <si>
-    <t>C:\Users\loren\Politecnico di Milano\DENG-SESAM - Documenti\DATASETS\Exiobase 3.8.2\MRSUT\MRSUT_2011.zip</t>
-  </si>
-  <si>
     <t>Results</t>
   </si>
   <si>
-    <t>C:\Users\loren\Politecnico di Milano\DENG-SESAM - Documenti\DATASETS\Exiobase 3.8.2\IOT\IOT_2011_ixi.zip</t>
-  </si>
-  <si>
     <t>Database</t>
   </si>
   <si>
@@ -70,6 +64,24 @@
   </si>
   <si>
     <t>C:\Users\loren\Documents\GitHub\SESAM\GT-IOA\Plots</t>
+  </si>
+  <si>
+    <t>Electricity</t>
+  </si>
+  <si>
+    <t>C:\Users\loren\Politecnico di Milano\DENG-SESAM - Documenti\DATASETS\Exiobase Hybrid 3.3.18</t>
+  </si>
+  <si>
+    <t>EXIOBASE Hybrid</t>
+  </si>
+  <si>
+    <t>C:\Users\loren\Politecnico di Milano\DENG-SESAM - Documenti\DATASETS\Exiobase 3.8.2\MRSUT</t>
+  </si>
+  <si>
+    <t>C:\Users\loren\Politecnico di Milano\DENG-SESAM - Documenti\DATASETS\Exiobase 3.8.2\IOT</t>
+  </si>
+  <si>
+    <t>C:\Users\loren\Documents\GitHub\SESAM\GT-IOA\Shocks\Electricity price logics\ShockMaster.xlsx</t>
   </si>
 </sst>
 </file>
@@ -107,7 +119,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -388,15 +400,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="105.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -407,62 +419,75 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
+      <c r="A4" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9" s="1"/>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New results by tech performance
</commit_message>
<xml_diff>
--- a/Paths.xlsx
+++ b/Paths.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\SESAM\GT-IOA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D49993F-94A0-4C1B-A88C-24DF4DEF2DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBBEF23C-5301-4899-B2B0-728A8F8839B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3855" yWindow="2925" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -66,9 +66,6 @@
     <t>C:\Users\loren\Documents\GitHub\SESAM\GT-IOA\Plots</t>
   </si>
   <si>
-    <t>Electricity</t>
-  </si>
-  <si>
     <t>C:\Users\loren\Politecnico di Milano\DENG-SESAM - Documenti\DATASETS\Exiobase Hybrid 3.3.18</t>
   </si>
   <si>
@@ -81,7 +78,10 @@
     <t>C:\Users\loren\Politecnico di Milano\DENG-SESAM - Documenti\DATASETS\Exiobase 3.8.2\IOT</t>
   </si>
   <si>
-    <t>C:\Users\loren\Documents\GitHub\SESAM\GT-IOA\Shocks\Electricity price logics\ShockMaster.xlsx</t>
+    <t>C:\Users\loren\Documents\GitHub\SESAM\GT-IOA\Shocks\ShockMaster.xlsx</t>
+  </si>
+  <si>
+    <t>ShockMaster</t>
   </si>
 </sst>
 </file>
@@ -402,8 +402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,7 +422,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -430,15 +430,15 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -483,10 +483,10 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>